<commit_message>
Added CRON, CSV file
</commit_message>
<xml_diff>
--- a/dane_pogodowe.xlsx
+++ b/dane_pogodowe.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,7 +700,1805 @@
         <v>1.34</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>45846.81753112444</v>
+        <v>45846.81753112269</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D9" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>45847.78429261574</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>45847.78447092592</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E11" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>45847.78464606481</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D12" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>45847.78482097222</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D13" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>45847.7849959838</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>45847.78517108796</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>45847.78534615741</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D16" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>45847.78552138889</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D17" t="n">
+        <v>100</v>
+      </c>
+      <c r="E17" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>45847.78569643519</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D18" t="n">
+        <v>100</v>
+      </c>
+      <c r="E18" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>45847.7858715625</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D19" t="n">
+        <v>100</v>
+      </c>
+      <c r="E19" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>45847.78604702546</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D20" t="n">
+        <v>100</v>
+      </c>
+      <c r="E20" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>45847.78622232639</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D21" t="n">
+        <v>100</v>
+      </c>
+      <c r="E21" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>45847.78639761574</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D22" t="n">
+        <v>100</v>
+      </c>
+      <c r="E22" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>45847.78657293982</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D23" t="n">
+        <v>100</v>
+      </c>
+      <c r="E23" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>45847.78674825231</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D24" t="n">
+        <v>100</v>
+      </c>
+      <c r="E24" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>45847.7869236574</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D25" t="n">
+        <v>100</v>
+      </c>
+      <c r="E25" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>45847.78709890047</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D26" t="n">
+        <v>100</v>
+      </c>
+      <c r="E26" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>45847.78727423611</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D27" t="n">
+        <v>100</v>
+      </c>
+      <c r="E27" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>45847.78744958333</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D28" t="n">
+        <v>100</v>
+      </c>
+      <c r="E28" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>45847.78762494213</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E29" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>45847.78780037037</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D30" t="n">
+        <v>100</v>
+      </c>
+      <c r="E30" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>45847.78797569445</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D31" t="n">
+        <v>100</v>
+      </c>
+      <c r="E31" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>moderate rain</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>45847.78815104167</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D32" t="n">
+        <v>100</v>
+      </c>
+      <c r="E32" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>45847.78832626157</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D33" t="n">
+        <v>100</v>
+      </c>
+      <c r="E33" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>45847.78850146991</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D34" t="n">
+        <v>100</v>
+      </c>
+      <c r="E34" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>45847.78867658565</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D35" t="n">
+        <v>100</v>
+      </c>
+      <c r="E35" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>45847.78885174768</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D36" t="n">
+        <v>100</v>
+      </c>
+      <c r="E36" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>45847.78902701389</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I37" s="2" t="n">
+        <v>45847.78920203703</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D38" t="n">
+        <v>100</v>
+      </c>
+      <c r="E38" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>45847.78937726852</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D39" t="n">
+        <v>100</v>
+      </c>
+      <c r="E39" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I39" s="2" t="n">
+        <v>45847.78955244213</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D40" t="n">
+        <v>100</v>
+      </c>
+      <c r="E40" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>45847.78972769676</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D41" t="n">
+        <v>100</v>
+      </c>
+      <c r="E41" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>45847.78990292824</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D42" t="n">
+        <v>100</v>
+      </c>
+      <c r="E42" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>45847.79007815972</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D43" t="n">
+        <v>100</v>
+      </c>
+      <c r="E43" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <v>45847.79025346065</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D44" t="n">
+        <v>100</v>
+      </c>
+      <c r="E44" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <v>45847.79042872685</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D45" t="n">
+        <v>100</v>
+      </c>
+      <c r="E45" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <v>45847.79060394676</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D46" t="n">
+        <v>100</v>
+      </c>
+      <c r="E46" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I46" s="2" t="n">
+        <v>45847.79077923611</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D47" t="n">
+        <v>100</v>
+      </c>
+      <c r="E47" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I47" s="2" t="n">
+        <v>45847.79095439815</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D48" t="n">
+        <v>100</v>
+      </c>
+      <c r="E48" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I48" s="2" t="n">
+        <v>45847.7911296875</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D49" t="n">
+        <v>100</v>
+      </c>
+      <c r="E49" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I49" s="2" t="n">
+        <v>45847.7913049074</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D50" t="n">
+        <v>100</v>
+      </c>
+      <c r="E50" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I50" s="2" t="n">
+        <v>45847.79148019676</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D51" t="n">
+        <v>100</v>
+      </c>
+      <c r="E51" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I51" s="2" t="n">
+        <v>45847.79165547454</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D52" t="n">
+        <v>100</v>
+      </c>
+      <c r="E52" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I52" s="2" t="n">
+        <v>45847.79183084491</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D53" t="n">
+        <v>100</v>
+      </c>
+      <c r="E53" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I53" s="2" t="n">
+        <v>45847.79200600694</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D54" t="n">
+        <v>100</v>
+      </c>
+      <c r="E54" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I54" s="2" t="n">
+        <v>45847.79221717593</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D55" t="n">
+        <v>100</v>
+      </c>
+      <c r="E55" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I55" s="2" t="n">
+        <v>45847.79239234954</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D56" t="n">
+        <v>100</v>
+      </c>
+      <c r="E56" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I56" s="2" t="n">
+        <v>45847.79256770833</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D57" t="n">
+        <v>100</v>
+      </c>
+      <c r="E57" t="n">
+        <v>284.8</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I57" s="2" t="n">
+        <v>45847.79274298611</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D58" t="n">
+        <v>100</v>
+      </c>
+      <c r="E58" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="I58" s="2" t="n">
+        <v>45847.79616098379</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D59" t="n">
+        <v>100</v>
+      </c>
+      <c r="E59" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="I59" s="2" t="n">
+        <v>45847.79633861111</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D60" t="n">
+        <v>100</v>
+      </c>
+      <c r="E60" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="I60" s="2" t="n">
+        <v>45847.79651393519</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D61" t="n">
+        <v>100</v>
+      </c>
+      <c r="E61" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="I61" s="2" t="n">
+        <v>45847.79668909722</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E62" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>9.539999999999999</v>
+      </c>
+      <c r="I62" s="2" t="n">
+        <v>45847.80455789352</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D63" t="n">
+        <v>100</v>
+      </c>
+      <c r="E63" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>9.539999999999999</v>
+      </c>
+      <c r="I63" s="2" t="n">
+        <v>45847.80584159722</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D64" t="n">
+        <v>100</v>
+      </c>
+      <c r="E64" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>9.539999999999999</v>
+      </c>
+      <c r="I64" s="2" t="n">
+        <v>45847.80601921296</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D65" t="n">
+        <v>100</v>
+      </c>
+      <c r="E65" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>9.539999999999999</v>
+      </c>
+      <c r="I65" s="2" t="n">
+        <v>45847.80619458333</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="n">
+        <v>284.63</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D66" t="n">
+        <v>100</v>
+      </c>
+      <c r="E66" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>light rain</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Wadowice</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>9.539999999999999</v>
+      </c>
+      <c r="I66" s="2" t="n">
+        <v>45847.80636991774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>